<commit_message>
debug perosnnel import debug personnel temp
</commit_message>
<xml_diff>
--- a/Web/wwwroot/Files/Template/Personnel_temp.xlsx
+++ b/Web/wwwroot/Files/Template/Personnel_temp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erfan Shayegh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erfan Shayegh\source\repos\IEfiwm\SalaryManagment\Web\wwwroot\Files\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$WWY$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$WWZ$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>كد پرسنلی</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>تعداد فرزندان</t>
+  </si>
+  <si>
+    <t>وضعیت کارمند</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -237,19 +240,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,1392 +539,1396 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ158"/>
+  <dimension ref="A1:AK158"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="AB1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AH5" sqref="AH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.77734375" style="1"/>
-    <col min="2" max="3" width="25.77734375" style="6"/>
+    <col min="2" max="3" width="25.77734375" style="5"/>
     <col min="4" max="16" width="25.77734375" style="1"/>
     <col min="17" max="17" width="25.77734375" style="3"/>
     <col min="18" max="24" width="25.77734375" style="1"/>
     <col min="25" max="25" width="59.109375" style="1" customWidth="1"/>
     <col min="26" max="26" width="25.77734375" style="1"/>
-    <col min="27" max="27" width="25.77734375" style="7"/>
-    <col min="28" max="31" width="25.77734375" style="1"/>
-    <col min="32" max="32" width="25.77734375" style="4"/>
-    <col min="33" max="16384" width="25.77734375" style="1"/>
+    <col min="27" max="27" width="25.77734375" style="6"/>
+    <col min="28" max="30" width="25.77734375" style="1"/>
+    <col min="31" max="32" width="25.77734375" style="1" customWidth="1"/>
+    <col min="33" max="33" width="25.77734375" style="4"/>
+    <col min="34" max="16384" width="25.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:37" s="8" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AA1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AD1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AE1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="10" t="s">
+      <c r="AF1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AH1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AI1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="11" t="s">
+      <c r="AK1" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N2" s="3"/>
       <c r="Q2" s="1"/>
       <c r="Y2" s="2"/>
-      <c r="AA2" s="6"/>
+      <c r="AA2" s="5"/>
       <c r="AD2" s="4"/>
-      <c r="AF2" s="1"/>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG2" s="1"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N3" s="3"/>
       <c r="Q3" s="1"/>
       <c r="Y3" s="2"/>
-      <c r="AA3" s="6"/>
+      <c r="AA3" s="5"/>
       <c r="AD3" s="4"/>
-      <c r="AF3" s="1"/>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG3" s="1"/>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N4" s="3"/>
       <c r="Q4" s="1"/>
       <c r="Y4" s="2"/>
-      <c r="AA4" s="6"/>
+      <c r="AA4" s="5"/>
       <c r="AD4" s="4"/>
-      <c r="AF4" s="1"/>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG4" s="1"/>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N5" s="3"/>
       <c r="Q5" s="1"/>
       <c r="Y5" s="2"/>
-      <c r="AA5" s="6"/>
+      <c r="AA5" s="5"/>
       <c r="AD5" s="4"/>
-      <c r="AF5" s="1"/>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG5" s="1"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N6" s="3"/>
       <c r="Q6" s="1"/>
       <c r="Y6" s="2"/>
-      <c r="AA6" s="6"/>
+      <c r="AA6" s="5"/>
       <c r="AD6" s="4"/>
-      <c r="AF6" s="1"/>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG6" s="1"/>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N7" s="3"/>
       <c r="Q7" s="1"/>
       <c r="Y7" s="2"/>
-      <c r="AA7" s="6"/>
+      <c r="AA7" s="5"/>
       <c r="AD7" s="4"/>
-      <c r="AF7" s="1"/>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG7" s="1"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N8" s="3"/>
       <c r="Q8" s="1"/>
       <c r="Y8" s="2"/>
-      <c r="AA8" s="6"/>
+      <c r="AA8" s="5"/>
       <c r="AD8" s="4"/>
-      <c r="AF8" s="1"/>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG8" s="1"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N9" s="3"/>
       <c r="Q9" s="1"/>
       <c r="Y9" s="2"/>
-      <c r="AA9" s="6"/>
+      <c r="AA9" s="5"/>
       <c r="AD9" s="4"/>
-      <c r="AF9" s="1"/>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG9" s="1"/>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N10" s="3"/>
       <c r="Q10" s="1"/>
       <c r="Y10" s="2"/>
-      <c r="AA10" s="6"/>
+      <c r="AA10" s="5"/>
       <c r="AD10" s="4"/>
-      <c r="AF10" s="1"/>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG10" s="1"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N11" s="3"/>
       <c r="Q11" s="1"/>
       <c r="Y11" s="2"/>
-      <c r="AA11" s="6"/>
+      <c r="AA11" s="5"/>
       <c r="AD11" s="4"/>
-      <c r="AF11" s="1"/>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG11" s="1"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N12" s="3"/>
       <c r="Q12" s="1"/>
       <c r="Y12" s="2"/>
-      <c r="AA12" s="6"/>
+      <c r="AA12" s="5"/>
       <c r="AD12" s="4"/>
-      <c r="AF12" s="1"/>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG12" s="1"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N13" s="3"/>
       <c r="Q13" s="1"/>
       <c r="Y13" s="2"/>
-      <c r="AA13" s="6"/>
+      <c r="AA13" s="5"/>
       <c r="AD13" s="4"/>
-      <c r="AF13" s="1"/>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG13" s="1"/>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N14" s="3"/>
       <c r="Q14" s="1"/>
       <c r="Y14" s="2"/>
-      <c r="AA14" s="6"/>
+      <c r="AA14" s="5"/>
       <c r="AD14" s="4"/>
-      <c r="AF14" s="1"/>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG14" s="1"/>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N15" s="3"/>
       <c r="Q15" s="1"/>
       <c r="Y15" s="2"/>
-      <c r="AA15" s="6"/>
+      <c r="AA15" s="5"/>
       <c r="AD15" s="4"/>
-      <c r="AF15" s="1"/>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AG15" s="1"/>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="N16" s="3"/>
       <c r="Q16" s="1"/>
       <c r="Y16" s="2"/>
-      <c r="AA16" s="6"/>
+      <c r="AA16" s="5"/>
       <c r="AD16" s="4"/>
-      <c r="AF16" s="1"/>
-    </row>
-    <row r="17" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG16" s="1"/>
+    </row>
+    <row r="17" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N17" s="3"/>
       <c r="Q17" s="1"/>
       <c r="Y17" s="2"/>
-      <c r="AA17" s="6"/>
+      <c r="AA17" s="5"/>
       <c r="AD17" s="4"/>
-      <c r="AF17" s="1"/>
-    </row>
-    <row r="18" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG17" s="1"/>
+    </row>
+    <row r="18" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N18" s="3"/>
       <c r="Q18" s="1"/>
       <c r="Y18" s="2"/>
-      <c r="AA18" s="6"/>
+      <c r="AA18" s="5"/>
       <c r="AD18" s="4"/>
-      <c r="AF18" s="1"/>
-    </row>
-    <row r="19" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG18" s="1"/>
+    </row>
+    <row r="19" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N19" s="3"/>
       <c r="Q19" s="1"/>
       <c r="Y19" s="2"/>
-      <c r="AA19" s="6"/>
+      <c r="AA19" s="5"/>
       <c r="AD19" s="4"/>
-      <c r="AF19" s="1"/>
-    </row>
-    <row r="20" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG19" s="1"/>
+    </row>
+    <row r="20" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N20" s="3"/>
       <c r="Q20" s="1"/>
       <c r="Y20" s="2"/>
-      <c r="AA20" s="6"/>
+      <c r="AA20" s="5"/>
       <c r="AD20" s="4"/>
-      <c r="AF20" s="1"/>
-    </row>
-    <row r="21" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG20" s="1"/>
+    </row>
+    <row r="21" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N21" s="3"/>
       <c r="Q21" s="1"/>
       <c r="Y21" s="2"/>
-      <c r="AA21" s="6"/>
+      <c r="AA21" s="5"/>
       <c r="AD21" s="4"/>
-      <c r="AF21" s="1"/>
-    </row>
-    <row r="22" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG21" s="1"/>
+    </row>
+    <row r="22" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N22" s="3"/>
       <c r="Q22" s="1"/>
       <c r="Y22" s="2"/>
-      <c r="AA22" s="6"/>
+      <c r="AA22" s="5"/>
       <c r="AD22" s="4"/>
-      <c r="AF22" s="1"/>
-    </row>
-    <row r="23" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG22" s="1"/>
+    </row>
+    <row r="23" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N23" s="3"/>
       <c r="Q23" s="1"/>
       <c r="Y23" s="2"/>
-      <c r="AA23" s="6"/>
+      <c r="AA23" s="5"/>
       <c r="AD23" s="4"/>
-      <c r="AF23" s="1"/>
-    </row>
-    <row r="24" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG23" s="1"/>
+    </row>
+    <row r="24" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N24" s="3"/>
       <c r="Q24" s="1"/>
       <c r="Y24" s="2"/>
-      <c r="AA24" s="6"/>
+      <c r="AA24" s="5"/>
       <c r="AD24" s="4"/>
-      <c r="AF24" s="1"/>
-    </row>
-    <row r="25" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG24" s="1"/>
+    </row>
+    <row r="25" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N25" s="3"/>
       <c r="Q25" s="1"/>
       <c r="Y25" s="2"/>
-      <c r="AA25" s="6"/>
+      <c r="AA25" s="5"/>
       <c r="AD25" s="4"/>
-      <c r="AF25" s="1"/>
-    </row>
-    <row r="26" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG25" s="1"/>
+    </row>
+    <row r="26" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N26" s="3"/>
       <c r="Q26" s="1"/>
       <c r="Y26" s="2"/>
-      <c r="AA26" s="6"/>
+      <c r="AA26" s="5"/>
       <c r="AD26" s="4"/>
-      <c r="AF26" s="1"/>
-    </row>
-    <row r="27" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG26" s="1"/>
+    </row>
+    <row r="27" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N27" s="3"/>
       <c r="Q27" s="1"/>
       <c r="Y27" s="2"/>
-      <c r="AA27" s="6"/>
+      <c r="AA27" s="5"/>
       <c r="AD27" s="4"/>
-      <c r="AF27" s="1"/>
-    </row>
-    <row r="28" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG27" s="1"/>
+    </row>
+    <row r="28" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N28" s="3"/>
       <c r="Q28" s="1"/>
       <c r="Y28" s="2"/>
-      <c r="AA28" s="6"/>
+      <c r="AA28" s="5"/>
       <c r="AD28" s="4"/>
-      <c r="AF28" s="1"/>
-    </row>
-    <row r="29" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG28" s="1"/>
+    </row>
+    <row r="29" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N29" s="3"/>
       <c r="Q29" s="1"/>
       <c r="Y29" s="2"/>
-      <c r="AA29" s="6"/>
+      <c r="AA29" s="5"/>
       <c r="AD29" s="4"/>
-      <c r="AF29" s="1"/>
-    </row>
-    <row r="30" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG29" s="1"/>
+    </row>
+    <row r="30" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N30" s="3"/>
       <c r="Q30" s="1"/>
       <c r="Y30" s="2"/>
-      <c r="AA30" s="6"/>
+      <c r="AA30" s="5"/>
       <c r="AD30" s="4"/>
-      <c r="AF30" s="1"/>
-    </row>
-    <row r="31" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG30" s="1"/>
+    </row>
+    <row r="31" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N31" s="3"/>
       <c r="Q31" s="1"/>
       <c r="Y31" s="2"/>
-      <c r="AA31" s="6"/>
+      <c r="AA31" s="5"/>
       <c r="AD31" s="4"/>
-      <c r="AF31" s="1"/>
-    </row>
-    <row r="32" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG31" s="1"/>
+    </row>
+    <row r="32" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N32" s="3"/>
       <c r="Q32" s="1"/>
       <c r="Y32" s="2"/>
-      <c r="AA32" s="6"/>
+      <c r="AA32" s="5"/>
       <c r="AD32" s="4"/>
-      <c r="AF32" s="1"/>
-    </row>
-    <row r="33" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG32" s="1"/>
+    </row>
+    <row r="33" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N33" s="3"/>
       <c r="Q33" s="1"/>
       <c r="Y33" s="2"/>
-      <c r="AA33" s="6"/>
+      <c r="AA33" s="5"/>
       <c r="AD33" s="4"/>
-      <c r="AF33" s="1"/>
-    </row>
-    <row r="34" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG33" s="1"/>
+    </row>
+    <row r="34" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N34" s="3"/>
       <c r="Q34" s="1"/>
       <c r="Y34" s="2"/>
-      <c r="AA34" s="6"/>
+      <c r="AA34" s="5"/>
       <c r="AD34" s="4"/>
-      <c r="AF34" s="1"/>
-    </row>
-    <row r="35" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG34" s="1"/>
+    </row>
+    <row r="35" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N35" s="3"/>
       <c r="Q35" s="1"/>
       <c r="Y35" s="2"/>
-      <c r="AA35" s="6"/>
+      <c r="AA35" s="5"/>
       <c r="AD35" s="4"/>
-      <c r="AF35" s="1"/>
-    </row>
-    <row r="36" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG35" s="1"/>
+    </row>
+    <row r="36" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N36" s="3"/>
       <c r="Q36" s="1"/>
       <c r="Y36" s="2"/>
-      <c r="AA36" s="6"/>
+      <c r="AA36" s="5"/>
       <c r="AD36" s="4"/>
-      <c r="AF36" s="1"/>
-    </row>
-    <row r="37" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG36" s="1"/>
+    </row>
+    <row r="37" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N37" s="3"/>
       <c r="Q37" s="1"/>
       <c r="Y37" s="2"/>
-      <c r="AA37" s="6"/>
+      <c r="AA37" s="5"/>
       <c r="AD37" s="4"/>
-      <c r="AF37" s="1"/>
-    </row>
-    <row r="38" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG37" s="1"/>
+    </row>
+    <row r="38" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N38" s="3"/>
       <c r="Q38" s="1"/>
       <c r="Y38" s="2"/>
-      <c r="AA38" s="6"/>
+      <c r="AA38" s="5"/>
       <c r="AD38" s="4"/>
-      <c r="AF38" s="1"/>
-    </row>
-    <row r="39" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG38" s="1"/>
+    </row>
+    <row r="39" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N39" s="3"/>
       <c r="Q39" s="1"/>
       <c r="Y39" s="2"/>
-      <c r="AA39" s="6"/>
+      <c r="AA39" s="5"/>
       <c r="AD39" s="4"/>
-      <c r="AF39" s="1"/>
-    </row>
-    <row r="40" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG39" s="1"/>
+    </row>
+    <row r="40" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N40" s="3"/>
       <c r="Q40" s="1"/>
       <c r="Y40" s="2"/>
-      <c r="AA40" s="6"/>
+      <c r="AA40" s="5"/>
       <c r="AD40" s="4"/>
-      <c r="AF40" s="1"/>
-    </row>
-    <row r="41" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG40" s="1"/>
+    </row>
+    <row r="41" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N41" s="3"/>
       <c r="Q41" s="1"/>
       <c r="Y41" s="2"/>
-      <c r="AA41" s="6"/>
+      <c r="AA41" s="5"/>
       <c r="AD41" s="4"/>
-      <c r="AF41" s="1"/>
-    </row>
-    <row r="42" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG41" s="1"/>
+    </row>
+    <row r="42" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N42" s="3"/>
       <c r="Q42" s="1"/>
       <c r="Y42" s="2"/>
-      <c r="AA42" s="6"/>
+      <c r="AA42" s="5"/>
       <c r="AD42" s="4"/>
-      <c r="AF42" s="1"/>
-    </row>
-    <row r="43" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG42" s="1"/>
+    </row>
+    <row r="43" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N43" s="3"/>
       <c r="Q43" s="1"/>
       <c r="Y43" s="2"/>
-      <c r="AA43" s="6"/>
+      <c r="AA43" s="5"/>
       <c r="AD43" s="4"/>
-      <c r="AF43" s="1"/>
-    </row>
-    <row r="44" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG43" s="1"/>
+    </row>
+    <row r="44" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N44" s="3"/>
       <c r="Q44" s="1"/>
       <c r="Y44" s="2"/>
-      <c r="AA44" s="6"/>
+      <c r="AA44" s="5"/>
       <c r="AD44" s="4"/>
-      <c r="AF44" s="1"/>
-    </row>
-    <row r="45" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG44" s="1"/>
+    </row>
+    <row r="45" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N45" s="3"/>
       <c r="Q45" s="1"/>
       <c r="Y45" s="2"/>
-      <c r="AA45" s="6"/>
+      <c r="AA45" s="5"/>
       <c r="AD45" s="4"/>
-      <c r="AF45" s="1"/>
-    </row>
-    <row r="46" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG45" s="1"/>
+    </row>
+    <row r="46" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N46" s="3"/>
       <c r="Q46" s="1"/>
       <c r="Y46" s="2"/>
-      <c r="AA46" s="6"/>
+      <c r="AA46" s="5"/>
       <c r="AD46" s="4"/>
-      <c r="AF46" s="1"/>
-    </row>
-    <row r="47" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG46" s="1"/>
+    </row>
+    <row r="47" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N47" s="3"/>
       <c r="Q47" s="1"/>
       <c r="Y47" s="2"/>
-      <c r="AA47" s="6"/>
+      <c r="AA47" s="5"/>
       <c r="AD47" s="4"/>
-      <c r="AF47" s="1"/>
-    </row>
-    <row r="48" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG47" s="1"/>
+    </row>
+    <row r="48" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N48" s="3"/>
       <c r="Q48" s="1"/>
       <c r="Y48" s="2"/>
-      <c r="AA48" s="6"/>
+      <c r="AA48" s="5"/>
       <c r="AD48" s="4"/>
-      <c r="AF48" s="1"/>
-    </row>
-    <row r="49" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG48" s="1"/>
+    </row>
+    <row r="49" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N49" s="3"/>
       <c r="Q49" s="1"/>
       <c r="Y49" s="2"/>
-      <c r="AA49" s="6"/>
+      <c r="AA49" s="5"/>
       <c r="AD49" s="4"/>
-      <c r="AF49" s="1"/>
-    </row>
-    <row r="50" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG49" s="1"/>
+    </row>
+    <row r="50" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N50" s="3"/>
       <c r="Q50" s="1"/>
       <c r="Y50" s="2"/>
-      <c r="AA50" s="6"/>
+      <c r="AA50" s="5"/>
       <c r="AD50" s="4"/>
-      <c r="AF50" s="1"/>
-    </row>
-    <row r="51" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG50" s="1"/>
+    </row>
+    <row r="51" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N51" s="3"/>
       <c r="Q51" s="1"/>
       <c r="Y51" s="2"/>
-      <c r="AA51" s="6"/>
+      <c r="AA51" s="5"/>
       <c r="AD51" s="4"/>
-      <c r="AF51" s="1"/>
-    </row>
-    <row r="52" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG51" s="1"/>
+    </row>
+    <row r="52" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N52" s="3"/>
       <c r="Q52" s="1"/>
       <c r="Y52" s="2"/>
-      <c r="AA52" s="6"/>
+      <c r="AA52" s="5"/>
       <c r="AD52" s="4"/>
-      <c r="AF52" s="1"/>
-    </row>
-    <row r="53" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG52" s="1"/>
+    </row>
+    <row r="53" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N53" s="3"/>
       <c r="Q53" s="1"/>
       <c r="Y53" s="2"/>
-      <c r="AA53" s="6"/>
+      <c r="AA53" s="5"/>
       <c r="AD53" s="4"/>
-      <c r="AF53" s="1"/>
-    </row>
-    <row r="54" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG53" s="1"/>
+    </row>
+    <row r="54" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N54" s="3"/>
       <c r="Q54" s="1"/>
       <c r="Y54" s="2"/>
-      <c r="AA54" s="6"/>
+      <c r="AA54" s="5"/>
       <c r="AD54" s="4"/>
-      <c r="AF54" s="1"/>
-    </row>
-    <row r="55" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG54" s="1"/>
+    </row>
+    <row r="55" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N55" s="3"/>
       <c r="Q55" s="1"/>
       <c r="Y55" s="2"/>
-      <c r="AA55" s="6"/>
+      <c r="AA55" s="5"/>
       <c r="AD55" s="4"/>
-      <c r="AF55" s="1"/>
-    </row>
-    <row r="56" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG55" s="1"/>
+    </row>
+    <row r="56" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N56" s="3"/>
       <c r="Q56" s="1"/>
       <c r="Y56" s="2"/>
-      <c r="AA56" s="6"/>
+      <c r="AA56" s="5"/>
       <c r="AD56" s="4"/>
-      <c r="AF56" s="1"/>
-    </row>
-    <row r="57" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG56" s="1"/>
+    </row>
+    <row r="57" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N57" s="3"/>
       <c r="Q57" s="1"/>
       <c r="Y57" s="2"/>
-      <c r="AA57" s="6"/>
+      <c r="AA57" s="5"/>
       <c r="AD57" s="4"/>
-      <c r="AF57" s="1"/>
-    </row>
-    <row r="58" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG57" s="1"/>
+    </row>
+    <row r="58" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N58" s="3"/>
       <c r="Q58" s="1"/>
       <c r="Y58" s="2"/>
-      <c r="AA58" s="6"/>
+      <c r="AA58" s="5"/>
       <c r="AD58" s="4"/>
-      <c r="AF58" s="1"/>
-    </row>
-    <row r="59" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG58" s="1"/>
+    </row>
+    <row r="59" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N59" s="3"/>
       <c r="Q59" s="1"/>
       <c r="Y59" s="2"/>
-      <c r="AA59" s="6"/>
+      <c r="AA59" s="5"/>
       <c r="AD59" s="4"/>
-      <c r="AF59" s="1"/>
-    </row>
-    <row r="60" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG59" s="1"/>
+    </row>
+    <row r="60" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N60" s="3"/>
       <c r="Q60" s="1"/>
       <c r="Y60" s="2"/>
-      <c r="AA60" s="6"/>
+      <c r="AA60" s="5"/>
       <c r="AD60" s="4"/>
-      <c r="AF60" s="1"/>
-    </row>
-    <row r="61" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG60" s="1"/>
+    </row>
+    <row r="61" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N61" s="3"/>
       <c r="Q61" s="1"/>
       <c r="Y61" s="2"/>
-      <c r="AA61" s="6"/>
+      <c r="AA61" s="5"/>
       <c r="AD61" s="4"/>
-      <c r="AF61" s="1"/>
-    </row>
-    <row r="62" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG61" s="1"/>
+    </row>
+    <row r="62" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N62" s="3"/>
       <c r="Q62" s="1"/>
       <c r="Y62" s="2"/>
-      <c r="AA62" s="6"/>
+      <c r="AA62" s="5"/>
       <c r="AD62" s="4"/>
-      <c r="AF62" s="1"/>
-    </row>
-    <row r="63" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG62" s="1"/>
+    </row>
+    <row r="63" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N63" s="3"/>
       <c r="Q63" s="1"/>
       <c r="Y63" s="2"/>
-      <c r="AA63" s="6"/>
+      <c r="AA63" s="5"/>
       <c r="AD63" s="4"/>
-      <c r="AF63" s="1"/>
-    </row>
-    <row r="64" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG63" s="1"/>
+    </row>
+    <row r="64" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N64" s="3"/>
       <c r="Q64" s="1"/>
       <c r="Y64" s="2"/>
-      <c r="AA64" s="6"/>
+      <c r="AA64" s="5"/>
       <c r="AD64" s="4"/>
-      <c r="AF64" s="1"/>
-    </row>
-    <row r="65" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG64" s="1"/>
+    </row>
+    <row r="65" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N65" s="3"/>
       <c r="Q65" s="1"/>
       <c r="Y65" s="2"/>
-      <c r="AA65" s="6"/>
+      <c r="AA65" s="5"/>
       <c r="AD65" s="4"/>
-      <c r="AF65" s="1"/>
-    </row>
-    <row r="66" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG65" s="1"/>
+    </row>
+    <row r="66" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N66" s="3"/>
       <c r="Q66" s="1"/>
       <c r="Y66" s="2"/>
-      <c r="AA66" s="6"/>
+      <c r="AA66" s="5"/>
       <c r="AD66" s="4"/>
-      <c r="AF66" s="1"/>
-    </row>
-    <row r="67" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG66" s="1"/>
+    </row>
+    <row r="67" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N67" s="3"/>
       <c r="Q67" s="1"/>
       <c r="Y67" s="2"/>
-      <c r="AA67" s="6"/>
+      <c r="AA67" s="5"/>
       <c r="AD67" s="4"/>
-      <c r="AF67" s="1"/>
-    </row>
-    <row r="68" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG67" s="1"/>
+    </row>
+    <row r="68" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N68" s="3"/>
       <c r="Q68" s="1"/>
       <c r="Y68" s="2"/>
-      <c r="AA68" s="6"/>
+      <c r="AA68" s="5"/>
       <c r="AD68" s="4"/>
-      <c r="AF68" s="1"/>
-    </row>
-    <row r="69" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG68" s="1"/>
+    </row>
+    <row r="69" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N69" s="3"/>
       <c r="Q69" s="1"/>
       <c r="Y69" s="2"/>
-      <c r="AA69" s="6"/>
+      <c r="AA69" s="5"/>
       <c r="AD69" s="4"/>
-      <c r="AF69" s="1"/>
-    </row>
-    <row r="70" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG69" s="1"/>
+    </row>
+    <row r="70" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N70" s="3"/>
       <c r="Q70" s="1"/>
       <c r="Y70" s="2"/>
-      <c r="AA70" s="6"/>
+      <c r="AA70" s="5"/>
       <c r="AD70" s="4"/>
-      <c r="AF70" s="1"/>
-    </row>
-    <row r="71" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG70" s="1"/>
+    </row>
+    <row r="71" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N71" s="3"/>
       <c r="Q71" s="1"/>
       <c r="Y71" s="2"/>
-      <c r="AA71" s="6"/>
+      <c r="AA71" s="5"/>
       <c r="AD71" s="4"/>
-      <c r="AF71" s="1"/>
-    </row>
-    <row r="72" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG71" s="1"/>
+    </row>
+    <row r="72" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N72" s="3"/>
       <c r="Q72" s="1"/>
       <c r="Y72" s="2"/>
-      <c r="AA72" s="6"/>
+      <c r="AA72" s="5"/>
       <c r="AD72" s="4"/>
-      <c r="AF72" s="1"/>
-    </row>
-    <row r="73" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG72" s="1"/>
+    </row>
+    <row r="73" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N73" s="3"/>
       <c r="Q73" s="1"/>
       <c r="Y73" s="2"/>
-      <c r="AA73" s="6"/>
+      <c r="AA73" s="5"/>
       <c r="AD73" s="4"/>
-      <c r="AF73" s="1"/>
-    </row>
-    <row r="74" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG73" s="1"/>
+    </row>
+    <row r="74" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N74" s="3"/>
       <c r="Q74" s="1"/>
       <c r="Y74" s="2"/>
-      <c r="AA74" s="6"/>
+      <c r="AA74" s="5"/>
       <c r="AD74" s="4"/>
-      <c r="AF74" s="1"/>
-    </row>
-    <row r="75" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG74" s="1"/>
+    </row>
+    <row r="75" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N75" s="3"/>
       <c r="Q75" s="1"/>
       <c r="Y75" s="2"/>
-      <c r="AA75" s="6"/>
+      <c r="AA75" s="5"/>
       <c r="AD75" s="4"/>
-      <c r="AF75" s="1"/>
-    </row>
-    <row r="76" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG75" s="1"/>
+    </row>
+    <row r="76" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N76" s="3"/>
       <c r="Q76" s="1"/>
       <c r="Y76" s="2"/>
-      <c r="AA76" s="6"/>
+      <c r="AA76" s="5"/>
       <c r="AD76" s="4"/>
-      <c r="AF76" s="1"/>
-    </row>
-    <row r="77" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG76" s="1"/>
+    </row>
+    <row r="77" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N77" s="3"/>
       <c r="Q77" s="1"/>
       <c r="Y77" s="2"/>
-      <c r="AA77" s="6"/>
+      <c r="AA77" s="5"/>
       <c r="AD77" s="4"/>
-      <c r="AF77" s="1"/>
-    </row>
-    <row r="78" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG77" s="1"/>
+    </row>
+    <row r="78" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N78" s="3"/>
       <c r="Q78" s="1"/>
       <c r="Y78" s="2"/>
-      <c r="AA78" s="6"/>
+      <c r="AA78" s="5"/>
       <c r="AD78" s="4"/>
-      <c r="AF78" s="1"/>
-    </row>
-    <row r="79" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG78" s="1"/>
+    </row>
+    <row r="79" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N79" s="3"/>
       <c r="Q79" s="1"/>
       <c r="Y79" s="2"/>
-      <c r="AA79" s="6"/>
+      <c r="AA79" s="5"/>
       <c r="AD79" s="4"/>
-      <c r="AF79" s="1"/>
-    </row>
-    <row r="80" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG79" s="1"/>
+    </row>
+    <row r="80" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N80" s="3"/>
       <c r="Q80" s="1"/>
       <c r="Y80" s="2"/>
-      <c r="AA80" s="6"/>
+      <c r="AA80" s="5"/>
       <c r="AD80" s="4"/>
-      <c r="AF80" s="1"/>
-    </row>
-    <row r="81" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG80" s="1"/>
+    </row>
+    <row r="81" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N81" s="3"/>
       <c r="Q81" s="1"/>
       <c r="Y81" s="2"/>
-      <c r="AA81" s="6"/>
+      <c r="AA81" s="5"/>
       <c r="AD81" s="4"/>
-      <c r="AF81" s="1"/>
-    </row>
-    <row r="82" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG81" s="1"/>
+    </row>
+    <row r="82" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N82" s="3"/>
       <c r="Q82" s="1"/>
       <c r="Y82" s="2"/>
-      <c r="AA82" s="6"/>
+      <c r="AA82" s="5"/>
       <c r="AD82" s="4"/>
-      <c r="AF82" s="1"/>
-    </row>
-    <row r="83" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG82" s="1"/>
+    </row>
+    <row r="83" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N83" s="3"/>
       <c r="Q83" s="1"/>
       <c r="Y83" s="2"/>
-      <c r="AA83" s="6"/>
+      <c r="AA83" s="5"/>
       <c r="AD83" s="4"/>
-      <c r="AF83" s="1"/>
-    </row>
-    <row r="84" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG83" s="1"/>
+    </row>
+    <row r="84" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N84" s="3"/>
       <c r="Q84" s="1"/>
       <c r="Y84" s="2"/>
-      <c r="AA84" s="6"/>
+      <c r="AA84" s="5"/>
       <c r="AD84" s="4"/>
-      <c r="AF84" s="1"/>
-    </row>
-    <row r="85" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG84" s="1"/>
+    </row>
+    <row r="85" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N85" s="3"/>
       <c r="Q85" s="1"/>
       <c r="Y85" s="2"/>
-      <c r="AA85" s="6"/>
+      <c r="AA85" s="5"/>
       <c r="AD85" s="4"/>
-      <c r="AF85" s="1"/>
-    </row>
-    <row r="86" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG85" s="1"/>
+    </row>
+    <row r="86" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N86" s="3"/>
       <c r="Q86" s="1"/>
       <c r="Y86" s="2"/>
-      <c r="AA86" s="6"/>
+      <c r="AA86" s="5"/>
       <c r="AD86" s="4"/>
-      <c r="AF86" s="1"/>
-    </row>
-    <row r="87" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG86" s="1"/>
+    </row>
+    <row r="87" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N87" s="3"/>
       <c r="Q87" s="1"/>
       <c r="Y87" s="2"/>
-      <c r="AA87" s="6"/>
+      <c r="AA87" s="5"/>
       <c r="AD87" s="4"/>
-      <c r="AF87" s="1"/>
-    </row>
-    <row r="88" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG87" s="1"/>
+    </row>
+    <row r="88" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N88" s="3"/>
       <c r="Q88" s="1"/>
       <c r="Y88" s="2"/>
-      <c r="AA88" s="6"/>
+      <c r="AA88" s="5"/>
       <c r="AD88" s="4"/>
-      <c r="AF88" s="1"/>
-    </row>
-    <row r="89" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG88" s="1"/>
+    </row>
+    <row r="89" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N89" s="3"/>
       <c r="Q89" s="1"/>
       <c r="Y89" s="2"/>
-      <c r="AA89" s="6"/>
+      <c r="AA89" s="5"/>
       <c r="AD89" s="4"/>
-      <c r="AF89" s="1"/>
-    </row>
-    <row r="90" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG89" s="1"/>
+    </row>
+    <row r="90" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N90" s="3"/>
       <c r="Q90" s="1"/>
       <c r="Y90" s="2"/>
-      <c r="AA90" s="6"/>
+      <c r="AA90" s="5"/>
       <c r="AD90" s="4"/>
-      <c r="AF90" s="1"/>
-    </row>
-    <row r="91" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG90" s="1"/>
+    </row>
+    <row r="91" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N91" s="3"/>
       <c r="Q91" s="1"/>
       <c r="Y91" s="2"/>
-      <c r="AA91" s="6"/>
+      <c r="AA91" s="5"/>
       <c r="AD91" s="4"/>
-      <c r="AF91" s="1"/>
-    </row>
-    <row r="92" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG91" s="1"/>
+    </row>
+    <row r="92" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N92" s="3"/>
       <c r="Q92" s="1"/>
       <c r="Y92" s="2"/>
-      <c r="AA92" s="6"/>
+      <c r="AA92" s="5"/>
       <c r="AD92" s="4"/>
-      <c r="AF92" s="1"/>
-    </row>
-    <row r="93" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG92" s="1"/>
+    </row>
+    <row r="93" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N93" s="3"/>
       <c r="Q93" s="1"/>
       <c r="Y93" s="2"/>
-      <c r="AA93" s="6"/>
+      <c r="AA93" s="5"/>
       <c r="AD93" s="4"/>
-      <c r="AF93" s="1"/>
-    </row>
-    <row r="94" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG93" s="1"/>
+    </row>
+    <row r="94" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N94" s="3"/>
       <c r="Q94" s="1"/>
       <c r="Y94" s="2"/>
-      <c r="AA94" s="6"/>
+      <c r="AA94" s="5"/>
       <c r="AD94" s="4"/>
-      <c r="AF94" s="1"/>
-    </row>
-    <row r="95" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG94" s="1"/>
+    </row>
+    <row r="95" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N95" s="3"/>
       <c r="Q95" s="1"/>
       <c r="Y95" s="2"/>
-      <c r="AA95" s="6"/>
+      <c r="AA95" s="5"/>
       <c r="AD95" s="4"/>
-      <c r="AF95" s="1"/>
-    </row>
-    <row r="96" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG95" s="1"/>
+    </row>
+    <row r="96" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N96" s="3"/>
       <c r="Q96" s="1"/>
       <c r="Y96" s="2"/>
-      <c r="AA96" s="6"/>
+      <c r="AA96" s="5"/>
       <c r="AD96" s="4"/>
-      <c r="AF96" s="1"/>
-    </row>
-    <row r="97" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG96" s="1"/>
+    </row>
+    <row r="97" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N97" s="3"/>
       <c r="Q97" s="1"/>
       <c r="Y97" s="2"/>
-      <c r="AA97" s="6"/>
+      <c r="AA97" s="5"/>
       <c r="AD97" s="4"/>
-      <c r="AF97" s="1"/>
-    </row>
-    <row r="98" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG97" s="1"/>
+    </row>
+    <row r="98" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N98" s="3"/>
       <c r="Q98" s="1"/>
       <c r="Y98" s="2"/>
-      <c r="AA98" s="6"/>
+      <c r="AA98" s="5"/>
       <c r="AD98" s="4"/>
-      <c r="AF98" s="1"/>
-    </row>
-    <row r="99" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG98" s="1"/>
+    </row>
+    <row r="99" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N99" s="3"/>
       <c r="Q99" s="1"/>
       <c r="Y99" s="2"/>
-      <c r="AA99" s="6"/>
+      <c r="AA99" s="5"/>
       <c r="AD99" s="4"/>
-      <c r="AF99" s="1"/>
-    </row>
-    <row r="100" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG99" s="1"/>
+    </row>
+    <row r="100" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N100" s="3"/>
       <c r="Q100" s="1"/>
       <c r="Y100" s="2"/>
-      <c r="AA100" s="6"/>
+      <c r="AA100" s="5"/>
       <c r="AD100" s="4"/>
-      <c r="AF100" s="1"/>
-    </row>
-    <row r="101" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG100" s="1"/>
+    </row>
+    <row r="101" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N101" s="3"/>
       <c r="Q101" s="1"/>
       <c r="Y101" s="2"/>
-      <c r="AA101" s="6"/>
+      <c r="AA101" s="5"/>
       <c r="AD101" s="4"/>
-      <c r="AF101" s="1"/>
-    </row>
-    <row r="102" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG101" s="1"/>
+    </row>
+    <row r="102" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N102" s="3"/>
       <c r="Q102" s="1"/>
       <c r="Y102" s="2"/>
-      <c r="AA102" s="6"/>
+      <c r="AA102" s="5"/>
       <c r="AD102" s="4"/>
-      <c r="AF102" s="1"/>
-    </row>
-    <row r="103" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG102" s="1"/>
+    </row>
+    <row r="103" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N103" s="3"/>
       <c r="Q103" s="1"/>
       <c r="Y103" s="2"/>
-      <c r="AA103" s="6"/>
+      <c r="AA103" s="5"/>
       <c r="AD103" s="4"/>
-      <c r="AF103" s="1"/>
-    </row>
-    <row r="104" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG103" s="1"/>
+    </row>
+    <row r="104" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N104" s="3"/>
       <c r="Q104" s="1"/>
       <c r="Y104" s="2"/>
-      <c r="AA104" s="6"/>
+      <c r="AA104" s="5"/>
       <c r="AD104" s="4"/>
-      <c r="AF104" s="1"/>
-    </row>
-    <row r="105" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG104" s="1"/>
+    </row>
+    <row r="105" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N105" s="3"/>
       <c r="Q105" s="1"/>
       <c r="Y105" s="2"/>
-      <c r="AA105" s="6"/>
+      <c r="AA105" s="5"/>
       <c r="AD105" s="4"/>
-      <c r="AF105" s="1"/>
-    </row>
-    <row r="106" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG105" s="1"/>
+    </row>
+    <row r="106" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N106" s="3"/>
       <c r="Q106" s="1"/>
       <c r="Y106" s="2"/>
-      <c r="AA106" s="6"/>
+      <c r="AA106" s="5"/>
       <c r="AD106" s="4"/>
-      <c r="AF106" s="1"/>
-    </row>
-    <row r="107" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG106" s="1"/>
+    </row>
+    <row r="107" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N107" s="3"/>
       <c r="Q107" s="1"/>
       <c r="Y107" s="2"/>
-      <c r="AA107" s="6"/>
+      <c r="AA107" s="5"/>
       <c r="AD107" s="4"/>
-      <c r="AF107" s="1"/>
-    </row>
-    <row r="108" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG107" s="1"/>
+    </row>
+    <row r="108" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N108" s="3"/>
       <c r="Q108" s="1"/>
       <c r="Y108" s="2"/>
-      <c r="AA108" s="6"/>
+      <c r="AA108" s="5"/>
       <c r="AD108" s="4"/>
-      <c r="AF108" s="1"/>
-    </row>
-    <row r="109" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG108" s="1"/>
+    </row>
+    <row r="109" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N109" s="3"/>
       <c r="Q109" s="1"/>
       <c r="Y109" s="2"/>
-      <c r="AA109" s="6"/>
+      <c r="AA109" s="5"/>
       <c r="AD109" s="4"/>
-      <c r="AF109" s="1"/>
-    </row>
-    <row r="110" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG109" s="1"/>
+    </row>
+    <row r="110" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N110" s="3"/>
       <c r="Q110" s="1"/>
       <c r="Y110" s="2"/>
-      <c r="AA110" s="6"/>
+      <c r="AA110" s="5"/>
       <c r="AD110" s="4"/>
-      <c r="AF110" s="1"/>
-    </row>
-    <row r="111" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG110" s="1"/>
+    </row>
+    <row r="111" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N111" s="3"/>
       <c r="Q111" s="1"/>
       <c r="Y111" s="2"/>
-      <c r="AA111" s="6"/>
+      <c r="AA111" s="5"/>
       <c r="AD111" s="4"/>
-      <c r="AF111" s="1"/>
-    </row>
-    <row r="112" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG111" s="1"/>
+    </row>
+    <row r="112" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N112" s="3"/>
       <c r="Q112" s="1"/>
       <c r="Y112" s="2"/>
-      <c r="AA112" s="6"/>
+      <c r="AA112" s="5"/>
       <c r="AD112" s="4"/>
-      <c r="AF112" s="1"/>
-    </row>
-    <row r="113" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG112" s="1"/>
+    </row>
+    <row r="113" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N113" s="3"/>
       <c r="Q113" s="1"/>
       <c r="Y113" s="2"/>
-      <c r="AA113" s="6"/>
+      <c r="AA113" s="5"/>
       <c r="AD113" s="4"/>
-      <c r="AF113" s="1"/>
-    </row>
-    <row r="114" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG113" s="1"/>
+    </row>
+    <row r="114" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N114" s="3"/>
       <c r="Q114" s="1"/>
       <c r="Y114" s="2"/>
-      <c r="AA114" s="6"/>
+      <c r="AA114" s="5"/>
       <c r="AD114" s="4"/>
-      <c r="AF114" s="1"/>
-    </row>
-    <row r="115" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG114" s="1"/>
+    </row>
+    <row r="115" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N115" s="3"/>
       <c r="Q115" s="1"/>
       <c r="Y115" s="2"/>
-      <c r="AA115" s="6"/>
+      <c r="AA115" s="5"/>
       <c r="AD115" s="4"/>
-      <c r="AF115" s="1"/>
-    </row>
-    <row r="116" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG115" s="1"/>
+    </row>
+    <row r="116" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N116" s="3"/>
       <c r="Q116" s="1"/>
       <c r="Y116" s="2"/>
-      <c r="AA116" s="6"/>
+      <c r="AA116" s="5"/>
       <c r="AD116" s="4"/>
-      <c r="AF116" s="1"/>
-    </row>
-    <row r="117" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG116" s="1"/>
+    </row>
+    <row r="117" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N117" s="3"/>
       <c r="Q117" s="1"/>
       <c r="Y117" s="2"/>
-      <c r="AA117" s="6"/>
+      <c r="AA117" s="5"/>
       <c r="AD117" s="4"/>
-      <c r="AF117" s="1"/>
-    </row>
-    <row r="118" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG117" s="1"/>
+    </row>
+    <row r="118" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N118" s="3"/>
       <c r="Q118" s="1"/>
       <c r="Y118" s="2"/>
-      <c r="AA118" s="6"/>
+      <c r="AA118" s="5"/>
       <c r="AD118" s="4"/>
-      <c r="AF118" s="1"/>
-    </row>
-    <row r="119" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG118" s="1"/>
+    </row>
+    <row r="119" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N119" s="3"/>
       <c r="Q119" s="1"/>
       <c r="Y119" s="2"/>
-      <c r="AA119" s="6"/>
+      <c r="AA119" s="5"/>
       <c r="AD119" s="4"/>
-      <c r="AF119" s="1"/>
-    </row>
-    <row r="120" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG119" s="1"/>
+    </row>
+    <row r="120" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N120" s="3"/>
       <c r="Q120" s="1"/>
       <c r="Y120" s="2"/>
-      <c r="AA120" s="6"/>
+      <c r="AA120" s="5"/>
       <c r="AD120" s="4"/>
-      <c r="AF120" s="1"/>
-    </row>
-    <row r="121" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG120" s="1"/>
+    </row>
+    <row r="121" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N121" s="3"/>
       <c r="Q121" s="1"/>
       <c r="Y121" s="2"/>
-      <c r="AA121" s="6"/>
+      <c r="AA121" s="5"/>
       <c r="AD121" s="4"/>
-      <c r="AF121" s="1"/>
-    </row>
-    <row r="122" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG121" s="1"/>
+    </row>
+    <row r="122" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N122" s="3"/>
       <c r="Q122" s="1"/>
       <c r="Y122" s="2"/>
-      <c r="AA122" s="6"/>
+      <c r="AA122" s="5"/>
       <c r="AD122" s="4"/>
-      <c r="AF122" s="1"/>
-    </row>
-    <row r="123" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG122" s="1"/>
+    </row>
+    <row r="123" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N123" s="3"/>
       <c r="Q123" s="1"/>
       <c r="Y123" s="2"/>
-      <c r="AA123" s="6"/>
+      <c r="AA123" s="5"/>
       <c r="AD123" s="4"/>
-      <c r="AF123" s="1"/>
-    </row>
-    <row r="124" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG123" s="1"/>
+    </row>
+    <row r="124" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N124" s="3"/>
       <c r="Q124" s="1"/>
       <c r="Y124" s="2"/>
-      <c r="AA124" s="6"/>
+      <c r="AA124" s="5"/>
       <c r="AD124" s="4"/>
-      <c r="AF124" s="1"/>
-    </row>
-    <row r="125" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG124" s="1"/>
+    </row>
+    <row r="125" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N125" s="3"/>
       <c r="Q125" s="1"/>
       <c r="Y125" s="2"/>
-      <c r="AA125" s="6"/>
+      <c r="AA125" s="5"/>
       <c r="AD125" s="4"/>
-      <c r="AF125" s="1"/>
-    </row>
-    <row r="126" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG125" s="1"/>
+    </row>
+    <row r="126" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N126" s="3"/>
       <c r="Q126" s="1"/>
       <c r="Y126" s="2"/>
-      <c r="AA126" s="6"/>
+      <c r="AA126" s="5"/>
       <c r="AD126" s="4"/>
-      <c r="AF126" s="1"/>
-    </row>
-    <row r="127" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG126" s="1"/>
+    </row>
+    <row r="127" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N127" s="3"/>
       <c r="Q127" s="1"/>
       <c r="Y127" s="2"/>
-      <c r="AA127" s="6"/>
+      <c r="AA127" s="5"/>
       <c r="AD127" s="4"/>
-      <c r="AF127" s="1"/>
-    </row>
-    <row r="128" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG127" s="1"/>
+    </row>
+    <row r="128" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N128" s="3"/>
       <c r="Q128" s="1"/>
       <c r="Y128" s="2"/>
-      <c r="AA128" s="6"/>
+      <c r="AA128" s="5"/>
       <c r="AD128" s="4"/>
-      <c r="AF128" s="1"/>
-    </row>
-    <row r="129" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG128" s="1"/>
+    </row>
+    <row r="129" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N129" s="3"/>
       <c r="Q129" s="1"/>
       <c r="Y129" s="2"/>
-      <c r="AA129" s="6"/>
+      <c r="AA129" s="5"/>
       <c r="AD129" s="4"/>
-      <c r="AF129" s="1"/>
-    </row>
-    <row r="130" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG129" s="1"/>
+    </row>
+    <row r="130" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N130" s="3"/>
       <c r="Q130" s="1"/>
       <c r="Y130" s="2"/>
-      <c r="AA130" s="6"/>
+      <c r="AA130" s="5"/>
       <c r="AD130" s="4"/>
-      <c r="AF130" s="1"/>
-    </row>
-    <row r="131" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG130" s="1"/>
+    </row>
+    <row r="131" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N131" s="3"/>
       <c r="Q131" s="1"/>
       <c r="Y131" s="2"/>
-      <c r="AA131" s="6"/>
+      <c r="AA131" s="5"/>
       <c r="AD131" s="4"/>
-      <c r="AF131" s="1"/>
-    </row>
-    <row r="132" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG131" s="1"/>
+    </row>
+    <row r="132" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N132" s="3"/>
       <c r="Q132" s="1"/>
       <c r="Y132" s="2"/>
-      <c r="AA132" s="6"/>
+      <c r="AA132" s="5"/>
       <c r="AD132" s="4"/>
-      <c r="AF132" s="1"/>
-    </row>
-    <row r="133" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG132" s="1"/>
+    </row>
+    <row r="133" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N133" s="3"/>
       <c r="Q133" s="1"/>
       <c r="Y133" s="2"/>
-      <c r="AA133" s="6"/>
+      <c r="AA133" s="5"/>
       <c r="AD133" s="4"/>
-      <c r="AF133" s="1"/>
-    </row>
-    <row r="134" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG133" s="1"/>
+    </row>
+    <row r="134" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N134" s="3"/>
       <c r="Q134" s="1"/>
       <c r="Y134" s="2"/>
-      <c r="AA134" s="6"/>
+      <c r="AA134" s="5"/>
       <c r="AD134" s="4"/>
-      <c r="AF134" s="1"/>
-    </row>
-    <row r="135" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG134" s="1"/>
+    </row>
+    <row r="135" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N135" s="3"/>
       <c r="Q135" s="1"/>
       <c r="Y135" s="2"/>
-      <c r="AA135" s="6"/>
+      <c r="AA135" s="5"/>
       <c r="AD135" s="4"/>
-      <c r="AF135" s="1"/>
-    </row>
-    <row r="136" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG135" s="1"/>
+    </row>
+    <row r="136" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N136" s="3"/>
       <c r="Q136" s="1"/>
       <c r="Y136" s="2"/>
-      <c r="AA136" s="6"/>
+      <c r="AA136" s="5"/>
       <c r="AD136" s="4"/>
-      <c r="AF136" s="1"/>
-    </row>
-    <row r="137" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG136" s="1"/>
+    </row>
+    <row r="137" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N137" s="3"/>
       <c r="Q137" s="1"/>
       <c r="Y137" s="2"/>
-      <c r="AA137" s="6"/>
+      <c r="AA137" s="5"/>
       <c r="AD137" s="4"/>
-      <c r="AF137" s="1"/>
-    </row>
-    <row r="138" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG137" s="1"/>
+    </row>
+    <row r="138" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N138" s="3"/>
       <c r="Q138" s="1"/>
       <c r="Y138" s="2"/>
-      <c r="AA138" s="6"/>
+      <c r="AA138" s="5"/>
       <c r="AD138" s="4"/>
-      <c r="AF138" s="1"/>
-    </row>
-    <row r="139" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG138" s="1"/>
+    </row>
+    <row r="139" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N139" s="3"/>
       <c r="Q139" s="1"/>
       <c r="Y139" s="2"/>
-      <c r="AA139" s="6"/>
+      <c r="AA139" s="5"/>
       <c r="AD139" s="4"/>
-      <c r="AF139" s="1"/>
-    </row>
-    <row r="140" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG139" s="1"/>
+    </row>
+    <row r="140" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N140" s="3"/>
       <c r="Q140" s="1"/>
       <c r="Y140" s="2"/>
-      <c r="AA140" s="6"/>
+      <c r="AA140" s="5"/>
       <c r="AD140" s="4"/>
-      <c r="AF140" s="1"/>
-    </row>
-    <row r="141" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG140" s="1"/>
+    </row>
+    <row r="141" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N141" s="3"/>
       <c r="Q141" s="1"/>
       <c r="Y141" s="2"/>
-      <c r="AA141" s="6"/>
+      <c r="AA141" s="5"/>
       <c r="AD141" s="4"/>
-      <c r="AF141" s="1"/>
-    </row>
-    <row r="142" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG141" s="1"/>
+    </row>
+    <row r="142" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N142" s="3"/>
       <c r="Q142" s="1"/>
       <c r="Y142" s="2"/>
-      <c r="AA142" s="6"/>
+      <c r="AA142" s="5"/>
       <c r="AD142" s="4"/>
-      <c r="AF142" s="1"/>
-    </row>
-    <row r="143" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG142" s="1"/>
+    </row>
+    <row r="143" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N143" s="3"/>
       <c r="Q143" s="1"/>
       <c r="Y143" s="2"/>
-      <c r="AA143" s="6"/>
+      <c r="AA143" s="5"/>
       <c r="AD143" s="4"/>
-      <c r="AF143" s="1"/>
-    </row>
-    <row r="144" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG143" s="1"/>
+    </row>
+    <row r="144" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N144" s="3"/>
       <c r="Q144" s="1"/>
       <c r="Y144" s="2"/>
-      <c r="AA144" s="6"/>
+      <c r="AA144" s="5"/>
       <c r="AD144" s="4"/>
-      <c r="AF144" s="1"/>
-    </row>
-    <row r="145" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG144" s="1"/>
+    </row>
+    <row r="145" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N145" s="3"/>
       <c r="Q145" s="1"/>
       <c r="Y145" s="2"/>
-      <c r="AA145" s="6"/>
+      <c r="AA145" s="5"/>
       <c r="AD145" s="4"/>
-      <c r="AF145" s="1"/>
-    </row>
-    <row r="146" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG145" s="1"/>
+    </row>
+    <row r="146" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N146" s="3"/>
       <c r="Q146" s="1"/>
       <c r="Y146" s="2"/>
-      <c r="AA146" s="6"/>
+      <c r="AA146" s="5"/>
       <c r="AD146" s="4"/>
-      <c r="AF146" s="1"/>
-    </row>
-    <row r="147" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG146" s="1"/>
+    </row>
+    <row r="147" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N147" s="3"/>
       <c r="Q147" s="1"/>
       <c r="Y147" s="2"/>
-      <c r="AA147" s="6"/>
+      <c r="AA147" s="5"/>
       <c r="AD147" s="4"/>
-      <c r="AF147" s="1"/>
-    </row>
-    <row r="148" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG147" s="1"/>
+    </row>
+    <row r="148" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N148" s="3"/>
       <c r="Q148" s="1"/>
       <c r="Y148" s="2"/>
-      <c r="AA148" s="6"/>
+      <c r="AA148" s="5"/>
       <c r="AD148" s="4"/>
-      <c r="AF148" s="1"/>
-    </row>
-    <row r="149" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG148" s="1"/>
+    </row>
+    <row r="149" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N149" s="3"/>
       <c r="Q149" s="1"/>
       <c r="Y149" s="2"/>
-      <c r="AA149" s="6"/>
+      <c r="AA149" s="5"/>
       <c r="AD149" s="4"/>
-      <c r="AF149" s="1"/>
-    </row>
-    <row r="150" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG149" s="1"/>
+    </row>
+    <row r="150" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N150" s="3"/>
       <c r="Q150" s="1"/>
       <c r="Y150" s="2"/>
-      <c r="AA150" s="6"/>
+      <c r="AA150" s="5"/>
       <c r="AD150" s="4"/>
-      <c r="AF150" s="1"/>
-    </row>
-    <row r="151" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG150" s="1"/>
+    </row>
+    <row r="151" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N151" s="3"/>
       <c r="Q151" s="1"/>
       <c r="Y151" s="2"/>
-      <c r="AA151" s="6"/>
+      <c r="AA151" s="5"/>
       <c r="AD151" s="4"/>
-      <c r="AF151" s="1"/>
-    </row>
-    <row r="152" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG151" s="1"/>
+    </row>
+    <row r="152" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N152" s="3"/>
       <c r="Q152" s="1"/>
       <c r="Y152" s="2"/>
-      <c r="AA152" s="6"/>
+      <c r="AA152" s="5"/>
       <c r="AD152" s="4"/>
-      <c r="AF152" s="1"/>
-    </row>
-    <row r="153" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG152" s="1"/>
+    </row>
+    <row r="153" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N153" s="3"/>
       <c r="Q153" s="1"/>
       <c r="Y153" s="2"/>
-      <c r="AA153" s="6"/>
+      <c r="AA153" s="5"/>
       <c r="AD153" s="4"/>
-      <c r="AF153" s="1"/>
-    </row>
-    <row r="154" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG153" s="1"/>
+    </row>
+    <row r="154" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N154" s="3"/>
       <c r="Q154" s="1"/>
       <c r="Y154" s="2"/>
-      <c r="AA154" s="6"/>
+      <c r="AA154" s="5"/>
       <c r="AD154" s="4"/>
-      <c r="AF154" s="1"/>
-    </row>
-    <row r="155" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG154" s="1"/>
+    </row>
+    <row r="155" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N155" s="3"/>
       <c r="Q155" s="1"/>
       <c r="Y155" s="2"/>
-      <c r="AA155" s="6"/>
+      <c r="AA155" s="5"/>
       <c r="AD155" s="4"/>
-      <c r="AF155" s="1"/>
-    </row>
-    <row r="156" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG155" s="1"/>
+    </row>
+    <row r="156" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N156" s="3"/>
       <c r="Q156" s="1"/>
       <c r="Y156" s="2"/>
-      <c r="AA156" s="6"/>
+      <c r="AA156" s="5"/>
       <c r="AD156" s="4"/>
-      <c r="AF156" s="1"/>
-    </row>
-    <row r="157" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG156" s="1"/>
+    </row>
+    <row r="157" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N157" s="3"/>
       <c r="Q157" s="1"/>
       <c r="Y157" s="2"/>
-      <c r="AA157" s="6"/>
+      <c r="AA157" s="5"/>
       <c r="AD157" s="4"/>
-      <c r="AF157" s="1"/>
-    </row>
-    <row r="158" spans="14:32" x14ac:dyDescent="0.3">
+      <c r="AG157" s="1"/>
+    </row>
+    <row r="158" spans="14:33" x14ac:dyDescent="0.3">
       <c r="N158" s="3"/>
       <c r="Q158" s="1"/>
       <c r="Y158" s="2"/>
-      <c r="AA158" s="6"/>
+      <c r="AA158" s="5"/>
       <c r="AD158" s="4"/>
-      <c r="AF158" s="1"/>
+      <c r="AG158" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
upadte personnel import add setaccess
</commit_message>
<xml_diff>
--- a/Web/wwwroot/Files/Template/Personnel_temp.xlsx
+++ b/Web/wwwroot/Files/Template/Personnel_temp.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$WWZ$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$WXA$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>كد پرسنلی</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>وضعیت کارمند</t>
+  </si>
+  <si>
+    <t>شماره شبا</t>
   </si>
 </sst>
 </file>
@@ -536,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK1"/>
+  <dimension ref="A1:AL1"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="AB1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AE6" sqref="AE6"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="L1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -558,7 +561,7 @@
     <col min="34" max="16384" width="25.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -602,72 +605,75 @@
         <v>13</v>
       </c>
       <c r="O1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AF1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AG1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AI1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="9" t="s">
+      <c r="AJ1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AK1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" s="9" t="s">
+      <c r="AL1" s="9" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>